<commit_message>
scripts for Supplementary Files
</commit_message>
<xml_diff>
--- a/supplementary/data5.xlsx
+++ b/supplementary/data5.xlsx
@@ -29,7 +29,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="61">
   <si>
-    <t>Supplemental Data 5: Kinetic simulation parameters and corresponding fit values</t>
+    <t>Supplementary File 5: Kinetic simulation parameters and corresponding fit values</t>
   </si>
   <si>
     <t>N</t>
@@ -947,7 +947,7 @@
         <v>0.0146</v>
       </c>
       <c r="D16">
-        <v>0.0151</v>
+        <v>0.015</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -955,13 +955,13 @@
         <v>43</v>
       </c>
       <c r="B17">
-        <v>0.3263</v>
+        <v>0.3262</v>
       </c>
       <c r="C17">
         <v>0.321</v>
       </c>
       <c r="D17">
-        <v>0.332</v>
+        <v>0.3317</v>
       </c>
     </row>
   </sheetData>
@@ -1177,10 +1177,10 @@
         <v>43</v>
       </c>
       <c r="B17">
-        <v>0.2128</v>
+        <v>0.2127</v>
       </c>
       <c r="C17">
-        <v>0.2111</v>
+        <v>0.211</v>
       </c>
       <c r="D17">
         <v>0.2144</v>
@@ -1405,7 +1405,7 @@
         <v>0.2252</v>
       </c>
       <c r="D17">
-        <v>0.2295</v>
+        <v>0.2294</v>
       </c>
     </row>
   </sheetData>
@@ -1843,13 +1843,13 @@
         <v>43</v>
       </c>
       <c r="B17">
-        <v>0.2873</v>
+        <v>0.2872</v>
       </c>
       <c r="C17">
-        <v>0.2834</v>
+        <v>0.2837</v>
       </c>
       <c r="D17">
-        <v>0.2911</v>
+        <v>0.2909</v>
       </c>
     </row>
   </sheetData>
@@ -2704,13 +2704,13 @@
         <v>43</v>
       </c>
       <c r="B17">
-        <v>0.2191</v>
+        <v>0.2192</v>
       </c>
       <c r="C17">
-        <v>0.2164</v>
+        <v>0.2162</v>
       </c>
       <c r="D17">
-        <v>0.222</v>
+        <v>0.2225</v>
       </c>
     </row>
   </sheetData>
@@ -2912,7 +2912,7 @@
         <v>42</v>
       </c>
       <c r="B16">
-        <v>0.006</v>
+        <v>0.0061</v>
       </c>
       <c r="C16">
         <v>0.0059</v>
@@ -2926,13 +2926,13 @@
         <v>43</v>
       </c>
       <c r="B17">
-        <v>0.2583</v>
+        <v>0.2584</v>
       </c>
       <c r="C17">
-        <v>0.2534</v>
+        <v>0.2539</v>
       </c>
       <c r="D17">
-        <v>0.263</v>
+        <v>0.2634</v>
       </c>
     </row>
   </sheetData>
@@ -3148,13 +3148,13 @@
         <v>43</v>
       </c>
       <c r="B17">
-        <v>0.3327</v>
+        <v>0.333</v>
       </c>
       <c r="C17">
         <v>0.3255</v>
       </c>
       <c r="D17">
-        <v>0.3395</v>
+        <v>0.34</v>
       </c>
     </row>
   </sheetData>
@@ -3359,7 +3359,7 @@
         <v>0.009299999999999999</v>
       </c>
       <c r="C16">
-        <v>0.0091</v>
+        <v>0.0092</v>
       </c>
       <c r="D16">
         <v>0.0095</v>
@@ -3370,13 +3370,13 @@
         <v>43</v>
       </c>
       <c r="B17">
-        <v>0.3967</v>
+        <v>0.3964</v>
       </c>
       <c r="C17">
-        <v>0.3876</v>
+        <v>0.3882</v>
       </c>
       <c r="D17">
-        <v>0.4058</v>
+        <v>0.4053</v>
       </c>
     </row>
   </sheetData>
@@ -3578,7 +3578,7 @@
         <v>42</v>
       </c>
       <c r="B16">
-        <v>0.009900000000000001</v>
+        <v>0.0098</v>
       </c>
       <c r="C16">
         <v>0.0097</v>
@@ -3592,13 +3592,13 @@
         <v>43</v>
       </c>
       <c r="B17">
-        <v>0.2179</v>
+        <v>0.2177</v>
       </c>
       <c r="C17">
-        <v>0.2157</v>
+        <v>0.2158</v>
       </c>
       <c r="D17">
-        <v>0.2201</v>
+        <v>0.2197</v>
       </c>
     </row>
   </sheetData>
@@ -3817,10 +3817,10 @@
         <v>0.2401</v>
       </c>
       <c r="C17">
-        <v>0.2373</v>
+        <v>0.237</v>
       </c>
       <c r="D17">
-        <v>0.2431</v>
+        <v>0.2433</v>
       </c>
     </row>
   </sheetData>
@@ -4028,7 +4028,7 @@
         <v>0.0127</v>
       </c>
       <c r="D16">
-        <v>0.013</v>
+        <v>0.0131</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -4039,10 +4039,10 @@
         <v>0.2852</v>
       </c>
       <c r="C17">
-        <v>0.2813</v>
+        <v>0.2814</v>
       </c>
       <c r="D17">
-        <v>0.2894</v>
+        <v>0.2899</v>
       </c>
     </row>
   </sheetData>

</xml_diff>